<commit_message>
Corrected date format error in xlsx files.
</commit_message>
<xml_diff>
--- a/results/test_crocus/test_crocus.xlsx
+++ b/results/test_crocus/test_crocus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucg\Documents\GitHub\CryoGrid\results\test_crocus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\thin\02_Code\Matlab\CryoGRID\CryoGrid_test_20191119\results\test_crocus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="134">
   <si>
     <t>OUT</t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>Suossjavri_WRF_Norstore_adapted2.mat</t>
+  </si>
+  <si>
+    <t>30.09.2011</t>
+  </si>
+  <si>
+    <t>30.10.2011</t>
   </si>
 </sst>
 </file>
@@ -741,7 +747,7 @@
   <dimension ref="A3:I143"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,8 +994,8 @@
       <c r="A29" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="1">
-        <v>40816</v>
+      <c r="B29" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="D29" t="s">
         <v>39</v>
@@ -999,8 +1005,8 @@
       <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="1">
-        <v>40846</v>
+      <c r="B30" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="D30" t="s">
         <v>41</v>

</xml_diff>